<commit_message>
docs: terminate second sprint
</commit_message>
<xml_diff>
--- a/docs/process/second-sprint-backlog.xlsx
+++ b/docs/process/second-sprint-backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t xml:space="preserve">Remaining effort at the end of the day ... </t>
   </si>
@@ -52,7 +52,7 @@
     <t>Sviluppo della regola di movimento orizzontale con Prolog</t>
   </si>
   <si>
-    <t>Cesario, Kentpayeva</t>
+    <t>Kentpayeva</t>
   </si>
   <si>
     <t>Sviluppo della regola di movimento verticale con Prolog</t>
@@ -64,10 +64,13 @@
     <t>Sviluppo della regola di movimento in avanti del Pedone</t>
   </si>
   <si>
+    <t>Derevyanchenko</t>
+  </si>
+  <si>
     <t>Sviluppo della regola di movimento ad L del Cavallo</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Felice</t>
   </si>
   <si>
     <t>Sviluppo della regola di movimento diagonale dell'Alfiere</t>
@@ -100,6 +103,9 @@
       </rPr>
       <t>En Passant</t>
     </r>
+  </si>
+  <si>
+    <t>?</t>
   </si>
   <si>
     <r>
@@ -150,6 +156,9 @@
   </si>
   <si>
     <t>Sviluppo del modello dello stato del gioco</t>
+  </si>
+  <si>
+    <t>Cesario</t>
   </si>
   <si>
     <t>Sviluppo dello storico delle mosse</t>
@@ -719,8 +728,12 @@
       <c r="E5" s="12">
         <v>4.0</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="F5" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
@@ -746,11 +759,21 @@
       <c r="E6" s="12">
         <v>3.0</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="F6" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G6" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H6" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="14"/>
@@ -773,11 +796,21 @@
       <c r="E7" s="12">
         <v>3.0</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
+      <c r="F7" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G7" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I7" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="14"/>
@@ -800,9 +833,15 @@
       <c r="E8" s="12">
         <v>3.0</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="F8" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="I8" s="12"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
@@ -822,14 +861,20 @@
         <v>16</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E9" s="12">
         <v>2.0</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="F9" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="I9" s="12"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
@@ -846,18 +891,26 @@
       <c r="A10" s="9"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="12">
         <v>3.0</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="F10" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G10" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H10" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -873,18 +926,26 @@
       <c r="A11" s="9"/>
       <c r="B11" s="17"/>
       <c r="C11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>11</v>
       </c>
       <c r="E11" s="12">
         <v>3.0</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="F11" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G11" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H11" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -900,7 +961,7 @@
       <c r="A12" s="9"/>
       <c r="B12" s="17"/>
       <c r="C12" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>13</v>
@@ -908,12 +969,24 @@
       <c r="E12" s="12">
         <v>3.0</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="13"/>
+      <c r="F12" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G12" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H12" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J12" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="L12" s="13"/>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
@@ -927,20 +1000,32 @@
       <c r="A13" s="9"/>
       <c r="B13" s="17"/>
       <c r="C13" s="20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E13" s="12">
         <v>3.0</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="13"/>
+      <c r="F13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J13" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="L13" s="13"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
@@ -954,19 +1039,29 @@
       <c r="A14" s="9"/>
       <c r="B14" s="17"/>
       <c r="C14" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E14" s="12">
         <v>3.0</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="F14" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H14" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="K14" s="12"/>
       <c r="L14" s="13"/>
       <c r="M14" s="14"/>
@@ -981,21 +1076,35 @@
       <c r="A15" s="9"/>
       <c r="B15" s="17"/>
       <c r="C15" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="12">
         <v>3.0</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="13"/>
+      <c r="F15" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G15" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H15" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I15" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J15" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="K15" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
@@ -1008,21 +1117,35 @@
       <c r="A16" s="9"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E16" s="12">
         <v>3.0</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
+      <c r="F16" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G16" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H16" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I16" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J16" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="K16" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="L16" s="12">
+        <v>3.0</v>
+      </c>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
@@ -1035,20 +1158,32 @@
       <c r="A17" s="9"/>
       <c r="B17" s="17"/>
       <c r="C17" s="20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17" s="12">
         <v>3.0</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="F17" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G17" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="J17" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="L17" s="12"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
@@ -1062,18 +1197,26 @@
       <c r="A18" s="9"/>
       <c r="B18" s="17"/>
       <c r="C18" s="18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="12">
         <v>3.0</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="F18" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="G18" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="H18" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -1089,21 +1232,35 @@
       <c r="A19" s="9"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E19" s="12">
         <v>2.0</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
+      <c r="F19" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G19" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="H19" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="I19" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="J19" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="K19" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="L19" s="12">
+        <v>2.0</v>
+      </c>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
@@ -1115,20 +1272,26 @@
     <row r="20">
       <c r="A20" s="9"/>
       <c r="B20" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E20" s="12">
         <v>2.0</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="F20" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G20" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
@@ -1145,18 +1308,26 @@
       <c r="A21" s="9"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E21" s="12">
         <v>2.0</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
+      <c r="F21" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="G21" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="H21" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
@@ -1172,18 +1343,26 @@
       <c r="A22" s="9"/>
       <c r="B22" s="23"/>
       <c r="C22" s="18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E22" s="12">
         <v>1.0</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
+      <c r="F22" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G22" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="H22" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
@@ -1198,24 +1377,38 @@
     <row r="23">
       <c r="A23" s="9"/>
       <c r="B23" s="15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E23" s="12">
         <v>1.0</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
+      <c r="F23" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G23" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="H23" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I23" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="J23" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="K23" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
@@ -1228,18 +1421,26 @@
       <c r="A24" s="9"/>
       <c r="B24" s="23"/>
       <c r="C24" s="18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E24" s="12">
         <v>1.0</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
+      <c r="F24" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>

</xml_diff>